<commit_message>
add test handle servo option
</commit_message>
<xml_diff>
--- a/Test Data/servo feedback data.xlsx
+++ b/Test Data/servo feedback data.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mli138/workspace/Safe_Cracker/Test Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794E2C63-452E-E64B-8F42-64468574197D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15530" windowHeight="12910"/>
+    <workbookView xWindow="5420" yWindow="6200" windowWidth="15540" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,12 +85,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -89,7 +107,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -232,6 +249,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E64E-8840-AE19-49205BB2E44B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -278,242 +300,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="1"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>voltage</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>127</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>157</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>172</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0.63500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.73799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.84499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.94499999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.054</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1559999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2569999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.3580000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4590000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5620000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.659</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.756</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.8540000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.952</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.048</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.14</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.1909999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="166959360"/>
-        <c:axId val="166982016"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="166959360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166982016"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="166982016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166959360"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -532,20 +318,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -555,36 +347,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -636,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,9 +431,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -704,6 +483,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -879,16 +675,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A6:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>17</v>
       </c>
@@ -904,7 +700,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+10</f>
         <v>27</v>
@@ -913,7 +709,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="0">A3+10</f>
         <v>37</v>
@@ -922,7 +718,7 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -931,7 +727,7 @@
         <v>0.94499999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -940,7 +736,7 @@
         <v>1.054</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -949,7 +745,7 @@
         <v>1.1559999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -958,7 +754,7 @@
         <v>1.2569999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -967,7 +763,7 @@
         <v>1.3580000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>97</v>
@@ -976,7 +772,7 @@
         <v>1.4590000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>107</v>
@@ -985,7 +781,7 @@
         <v>1.5620000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>117</v>
@@ -994,7 +790,7 @@
         <v>1.659</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>127</v>
@@ -1003,7 +799,7 @@
         <v>1.756</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>137</v>
@@ -1012,7 +808,7 @@
         <v>1.8540000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>147</v>
@@ -1021,7 +817,7 @@
         <v>1.952</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>157</v>
@@ -1030,7 +826,7 @@
         <v>2.048</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>167</v>
@@ -1039,7 +835,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>172</v>
       </c>
@@ -1054,24 +850,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>